<commit_message>
Corrected typo on attribute labelling, updated polarization doc with Stokes vector.
</commit_message>
<xml_diff>
--- a/ARPES/tabular-to-yaml/mpes-nexus_metadata_parameters_reviewed.xlsx
+++ b/ARPES/tabular-to-yaml/mpes-nexus_metadata_parameters_reviewed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="784" firstSheet="6" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="784" firstSheet="8" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="NXentry" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="606">
   <si>
     <t>Name</t>
   </si>
@@ -2607,9 +2607,6 @@
     <t>type:units</t>
   </si>
   <si>
-    <t>NXentry:NXinstrument:name:/@short_name</t>
-  </si>
-  <si>
     <t>Acronym or other shorthand name</t>
   </si>
   <si>
@@ -2666,7 +2663,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:name:/@short_name</t>
+      <t>NXelectronanalyser:fast_axes</t>
     </r>
   </si>
   <si>
@@ -2680,7 +2677,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:fast_axes</t>
+      <t>NXelectronanalyser:slow_axes</t>
     </r>
   </si>
   <si>
@@ -2694,7 +2691,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:slow_axes</t>
+      <t>NXelectronanalyser:temporal_resolution</t>
     </r>
   </si>
   <si>
@@ -2708,7 +2705,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:temporal_resolution</t>
+      <t>NXelectronanalyser:energy_resolution</t>
     </r>
   </si>
   <si>
@@ -2722,7 +2719,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:energy_resolution</t>
+      <t>NXelectronanalyser:spatial_resolution</t>
     </r>
   </si>
   <si>
@@ -2736,7 +2733,21 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:spatial_resolution</t>
+      <t>NXelectronanalyser:acquisition_mode</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXprocess:NXdetector:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>other_converts</t>
     </r>
   </si>
   <si>
@@ -2750,21 +2761,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:acquisition_mode</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXprocess:NXdetector:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>other_converts</t>
+      <t>NXelectronanalyser:NXcollectionlens:extractor_current</t>
     </r>
   </si>
   <si>
@@ -2778,7 +2775,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:extractor_current</t>
+      <t>NXelectronanalyser:NXcollectionlens:extractor_voltage</t>
     </r>
   </si>
   <si>
@@ -2792,7 +2789,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:extractor_voltage</t>
+      <t>NXelectronanalyser:NXcollectionlens:working_distance</t>
     </r>
   </si>
   <si>
@@ -2806,7 +2803,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:working_distance</t>
+      <t>NXelectronanalyser:NXcollectionlens:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>lens_mode</t>
     </r>
   </si>
   <si>
@@ -2820,7 +2826,174 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:</t>
+      <t>NXelectronanalyser:NXcollectionlens:lens_names</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:NXcollectionlens:lens_voltages</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:NXcollectionlens:projection</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:NXcollectionlens:magnification</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:NXcollectionlens:field_aperture</t>
+    </r>
+  </si>
+  <si>
+    <t>contrast_aperture</t>
+  </si>
+  <si>
+    <t>NXaperture</t>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:NXcollectionlens:contrast_aperture</t>
+    </r>
+  </si>
+  <si>
+    <t>The size and position of the field aperture inserted in the column</t>
+  </si>
+  <si>
+    <t>The size and postion of the contrast aperture inserted in the column.</t>
+  </si>
+  <si>
+    <t>scheme</t>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>:NXelectronanalyser:NXenergydispersion:scheme</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>:NXelectronanalyser:NXenergydispersion:pass_energy</t>
+    </r>
+  </si>
+  <si>
+    <t>entrance_slit</t>
+  </si>
+  <si>
+    <t>exit_slit</t>
+  </si>
+  <si>
+    <t>Size, position and shape of the entrance slits in dispersive analyzers</t>
+  </si>
+  <si>
+    <t>Size, position and shape of the exit slits in dispersive analyzer</t>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:NXenergydispersion:center_energy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:NXenergydispersion:exit_slit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:NXenergydispersion:</t>
     </r>
     <r>
       <rPr>
@@ -2829,7 +3002,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>lens_mode</t>
+      <t>diameter</t>
     </r>
   </si>
   <si>
@@ -2843,7 +3016,41 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:lens_names</t>
+      <t>NXelectronanalyser:NXenergydispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>entrance_slit</t>
+    </r>
+  </si>
+  <si>
+    <t>acquisition_mode</t>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>:NXelectronanalyser:NXenergydispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>acquisition_mode</t>
     </r>
   </si>
   <si>
@@ -2857,7 +3064,119 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:lens_voltages</t>
+      <t>NXelectronanalyser:NXenergydispersion:tof_distance</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>spin_filter_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>spin_filter_FoM</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>spin_filter_shermann_function</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>spin_scattering_energy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>spin_scattering_angle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>spin_target</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>spin_target_preparation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>spin_target_preparation_date</t>
     </r>
   </si>
   <si>
@@ -2871,7 +3190,25 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:projection</t>
+      <t>NXelectronanaliser:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXdetector:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>amplifier_type</t>
     </r>
   </si>
   <si>
@@ -2885,7 +3222,25 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:magnification</t>
+      <t>NXelectronanaliser:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXdetector:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>detector_type</t>
     </r>
   </si>
   <si>
@@ -2899,14 +3254,26 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:field_aperture</t>
-    </r>
-  </si>
-  <si>
-    <t>contrast_aperture</t>
-  </si>
-  <si>
-    <t>NXaperture</t>
+      <t>NXelectronanaliser:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXdetector:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>detector_voltage</t>
+    </r>
   </si>
   <si>
     <r>
@@ -2919,57 +3286,26 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXcollectionlens:contrast_aperture</t>
-    </r>
-  </si>
-  <si>
-    <t>The size and position of the field aperture inserted in the column</t>
-  </si>
-  <si>
-    <t>The size and postion of the contrast aperture inserted in the column.</t>
-  </si>
-  <si>
-    <t>scheme</t>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>:NXelectronanalyser:NXenergydispersion:scheme</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>:NXelectronanalyser:NXenergydispersion:pass_energy</t>
-    </r>
-  </si>
-  <si>
-    <t>entrance_slit</t>
-  </si>
-  <si>
-    <t>exit_slit</t>
-  </si>
-  <si>
-    <t>Size, position and shape of the entrance slits in dispersive analyzers</t>
-  </si>
-  <si>
-    <t>Size, position and shape of the exit slits in dispersive analyzer</t>
+      <t>NXelectronanaliser:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXdetector:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_size</t>
+    </r>
   </si>
   <si>
     <r>
@@ -2982,7 +3318,25 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXenergydispersion:center_energy</t>
+      <t>NXelectronanaliser:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXdetector:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_count</t>
     </r>
   </si>
   <si>
@@ -2996,21 +3350,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NXelectronanalyser:NXenergydispersion:exit_slit</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanalyser:NXenergydispersion:</t>
+      <t>NXelectronanaliser:</t>
     </r>
     <r>
       <rPr>
@@ -3019,203 +3359,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>diameter</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanalyser:NXenergydispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>entrance_slit</t>
-    </r>
-  </si>
-  <si>
-    <t>acquisition_mode</t>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>:NXelectronanalyser:NXenergydispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>acquisition_mode</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanalyser:NXenergydispersion:tof_distance</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>spin_filter_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>spin_filter_FoM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>spin_filter_shermann_function</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>spin_scattering_energy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>spin_scattering_angle</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>spin_target</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>spin_target_preparation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXelectronanalyser:NXspindispersion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>spin_target_preparation_date</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanaliser:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>NXdetector:</t>
     </r>
     <r>
@@ -3225,166 +3368,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>amplifier_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanaliser:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXdetector:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>detector_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanaliser:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXdetector:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>detector_voltage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanaliser:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXdetector:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>sensor_size</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanaliser:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXdetector:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>sensor_count</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXelectronanaliser:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NXdetector:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>sensor_pixel_size</t>
     </r>
   </si>
@@ -3395,14 +3378,136 @@
     <t>bias</t>
   </si>
   <si>
-    <t>NXentry:NXsample:electric_field:/@direction</t>
-  </si>
-  <si>
     <t>NXentry:NXsample:magnetic_field</t>
   </si>
   <si>
-    <r>
-      <t>NXentry:NXsample:magnetic_field:/@direction</t>
+    <t>incident_energy</t>
+  </si>
+  <si>
+    <t>NXentry:NXinstrument:NXbeam:incident_energy</t>
+  </si>
+  <si>
+    <t>incident_polarization</t>
+  </si>
+  <si>
+    <t>NXentry:NXinstrument:NXbeam:incident_polarization</t>
+  </si>
+  <si>
+    <t>extent</t>
+  </si>
+  <si>
+    <t>beam size vector</t>
+  </si>
+  <si>
+    <t>NXentry:NXinstrument:NXbeam:extent</t>
+  </si>
+  <si>
+    <t>flux incident on beam plane area</t>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:NXbeam:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>flux</t>
+    </r>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Dim</t>
+  </si>
+  <si>
+    <t>[1,4]</t>
+  </si>
+  <si>
+    <t>[1,2]</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>Average source power</t>
+  </si>
+  <si>
+    <t>NXentry:NXinstrument:NXsource:power</t>
+  </si>
+  <si>
+    <t>[1,nl]</t>
+  </si>
+  <si>
+    <t>[1,nfa]</t>
+  </si>
+  <si>
+    <t>[1,nsa]</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>Vector determining the direction of the electric field</t>
+  </si>
+  <si>
+    <t>Vector determining the direction of the magnetic field</t>
+  </si>
+  <si>
+    <t>Vector determining the direction of the stress field</t>
+  </si>
+  <si>
+    <t>[1,3]</t>
+  </si>
+  <si>
+    <t>[1,nkx]</t>
+  </si>
+  <si>
+    <t>[1,nky]</t>
+  </si>
+  <si>
+    <t>[1,ne]</t>
+  </si>
+  <si>
+    <t>[1,ntpp]</t>
+  </si>
+  <si>
+    <t>[1,nkx],[1,nkx]</t>
+  </si>
+  <si>
+    <t>[1,nky],[1,nky]</t>
+  </si>
+  <si>
+    <t>[1,ne],[1,ne]</t>
+  </si>
+  <si>
+    <t>[1,ntpp],[1,ntpp]</t>
+  </si>
+  <si>
+    <t>[1,nx],[1,nx]</t>
+  </si>
+  <si>
+    <t>[ndx,ndy]</t>
+  </si>
+  <si>
+    <t>[2,nsym]</t>
+  </si>
+  <si>
+    <t>[1,ncoeff]</t>
+  </si>
+  <si>
+    <t>[1,nfeat]</t>
+  </si>
+  <si>
+    <t>NXentry:NXsample:magnetic_field:\@direction</t>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXsample:magnetic_field:\@direction</t>
     </r>
     <r>
       <rPr>
@@ -3416,132 +3521,27 @@
     </r>
   </si>
   <si>
-    <t>NXentry:NXsample:magnetic_field:/@direction</t>
-  </si>
-  <si>
-    <t>incident_energy</t>
-  </si>
-  <si>
-    <t>NXentry:NXinstrument:NXbeam:incident_energy</t>
-  </si>
-  <si>
-    <t>incident_polarization</t>
-  </si>
-  <si>
-    <t>Incident polarization as a Jones vector (complex?)</t>
-  </si>
-  <si>
-    <t>NXentry:NXinstrument:NXbeam:incident_polarization</t>
-  </si>
-  <si>
-    <t>extent</t>
-  </si>
-  <si>
-    <t>beam size vector</t>
-  </si>
-  <si>
-    <t>NXentry:NXinstrument:NXbeam:extent</t>
-  </si>
-  <si>
-    <t>flux incident on beam plane area</t>
-  </si>
-  <si>
-    <r>
-      <t>NXentry:NXinstrument:NXbeam:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>flux</t>
-    </r>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Dim</t>
-  </si>
-  <si>
-    <t>[1,4]</t>
-  </si>
-  <si>
-    <t>[1,2]</t>
-  </si>
-  <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>Average source power</t>
-  </si>
-  <si>
-    <t>NXentry:NXinstrument:NXsource:power</t>
-  </si>
-  <si>
-    <t>[1,nl]</t>
-  </si>
-  <si>
-    <t>[1,nfa]</t>
-  </si>
-  <si>
-    <t>[1,nsa]</t>
-  </si>
-  <si>
-    <t>attribute</t>
-  </si>
-  <si>
-    <t>Vector determining the direction of the electric field</t>
-  </si>
-  <si>
-    <t>Vector determining the direction of the magnetic field</t>
-  </si>
-  <si>
-    <t>Vector determining the direction of the stress field</t>
-  </si>
-  <si>
-    <t>[1,3]</t>
-  </si>
-  <si>
-    <t>[1,nkx]</t>
-  </si>
-  <si>
-    <t>[1,nky]</t>
-  </si>
-  <si>
-    <t>[1,ne]</t>
-  </si>
-  <si>
-    <t>[1,ntpp]</t>
-  </si>
-  <si>
-    <t>[1,nkx],[1,nkx]</t>
-  </si>
-  <si>
-    <t>[1,nky],[1,nky]</t>
-  </si>
-  <si>
-    <t>[1,ne],[1,ne]</t>
-  </si>
-  <si>
-    <t>[1,ntpp],[1,ntpp]</t>
-  </si>
-  <si>
-    <t>[1,nx],[1,nx]</t>
-  </si>
-  <si>
-    <t>[ndx,ndy]</t>
-  </si>
-  <si>
-    <t>[2,nsym]</t>
-  </si>
-  <si>
-    <t>[1,ncoeff]</t>
-  </si>
-  <si>
-    <t>[1,nfeat]</t>
+    <t>NXentry:NXsample:electric_field:\@direction</t>
+  </si>
+  <si>
+    <t>NXentry:NXinstrument:name:\@short_name</t>
+  </si>
+  <si>
+    <t>Incident polarization as a Stokes vector</t>
+  </si>
+  <si>
+    <r>
+      <t>NXentry:NXinstrument:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NXelectronanalyser:name:\@short_name</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3956,7 +3956,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -3971,10 +3971,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -4420,7 +4420,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4439,7 +4439,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -4454,21 +4454,21 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>269</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -4491,7 +4491,7 @@
         <v>271</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>82</v>
@@ -4514,7 +4514,7 @@
         <v>273</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>82</v>
@@ -4531,17 +4531,17 @@
     </row>
     <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>539</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>351</v>
@@ -4555,17 +4555,17 @@
     </row>
     <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>540</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>542</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>492</v>
@@ -4585,7 +4585,7 @@
         <v>275</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
@@ -4602,13 +4602,13 @@
     </row>
     <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>277</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -4631,7 +4631,7 @@
         <v>279</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>85</v>
@@ -4689,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -4704,10 +4704,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -4718,7 +4718,7 @@
         <v>281</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -4741,7 +4741,7 @@
         <v>283</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>182</v>
@@ -4764,7 +4764,7 @@
         <v>285</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>182</v>
@@ -4787,7 +4787,7 @@
         <v>287</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>82</v>
@@ -4810,7 +4810,7 @@
         <v>289</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -4833,7 +4833,7 @@
         <v>291</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -4856,7 +4856,7 @@
         <v>293</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -4879,7 +4879,7 @@
         <v>295</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
@@ -4918,7 +4918,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -4933,10 +4933,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
@@ -4947,7 +4947,7 @@
         <v>297</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -4970,7 +4970,7 @@
         <v>299</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -4993,7 +4993,7 @@
         <v>301</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>252</v>
@@ -5016,7 +5016,7 @@
         <v>303</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>85</v>
@@ -5039,7 +5039,7 @@
         <v>305</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>306</v>
@@ -5062,7 +5062,7 @@
         <v>308</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
@@ -5094,8 +5094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5109,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -5124,10 +5124,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -5181,7 +5181,7 @@
         <v>314</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>315</v>
@@ -5500,15 +5500,17 @@
     </row>
     <row r="18" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>602</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>252</v>
+      </c>
       <c r="F18" s="2" t="s">
         <v>351</v>
       </c>
@@ -5516,7 +5518,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5527,7 +5529,7 @@
         <v>352</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>186</v>
@@ -5544,15 +5546,17 @@
     </row>
     <row r="20" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>601</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="F20" s="2" t="s">
         <v>351</v>
       </c>
@@ -5560,7 +5564,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5588,15 +5592,17 @@
     </row>
     <row r="22" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>600</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="F22" s="2" t="s">
         <v>351</v>
       </c>
@@ -5604,7 +5610,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -5678,7 +5684,7 @@
     </row>
     <row r="26" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>365</v>
@@ -5940,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -5955,10 +5961,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6073,7 +6079,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6096,7 +6102,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6119,7 +6125,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6142,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6166,7 +6172,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6190,7 +6196,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6214,7 +6220,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6238,7 +6244,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
@@ -6249,7 +6255,7 @@
         <v>430</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
@@ -6289,7 +6295,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -6304,10 +6310,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -6399,7 +6405,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -6422,7 +6428,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -6445,7 +6451,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -6500,7 +6506,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -6515,10 +6521,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6610,7 +6616,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -6633,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -6679,7 +6685,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -6706,7 +6712,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -6721,10 +6727,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6770,7 +6776,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -6793,7 +6799,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -6816,7 +6822,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6839,7 +6845,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -6917,7 +6923,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -6932,10 +6938,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -7117,7 +7123,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7136,7 +7142,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -7151,10 +7157,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -7183,13 +7189,13 @@
     </row>
     <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>503</v>
+        <v>603</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -7238,8 +7244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7259,7 +7265,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -7274,10 +7280,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -7443,13 +7449,13 @@
     </row>
     <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>108</v>
@@ -7692,7 +7698,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -7831,7 +7837,7 @@
         <v>2</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="66" x14ac:dyDescent="0.3">
@@ -7913,8 +7919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7934,7 +7940,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -7949,10 +7955,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -8026,13 +8032,13 @@
     </row>
     <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>82</v>
@@ -8047,15 +8053,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>571</v>
+        <v>604</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -8067,18 +8073,18 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
@@ -8090,7 +8096,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -8160,7 +8166,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -8214,10 +8220,10 @@
         <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>127</v>
@@ -8243,7 +8249,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8259,7 +8265,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -8274,10 +8280,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -8347,7 +8353,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -8359,7 +8365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -8374,7 +8380,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -8389,10 +8395,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -8750,7 +8756,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8770,7 +8776,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -8785,10 +8791,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -8799,7 +8805,7 @@
         <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -8823,7 +8829,7 @@
         <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -8840,12 +8846,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>582</v>
+      </c>
       <c r="B4" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>512</v>
+        <v>605</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -8869,7 +8877,7 @@
         <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
@@ -8893,7 +8901,7 @@
         <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>82</v>
@@ -8917,7 +8925,7 @@
         <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
@@ -8941,7 +8949,7 @@
         <v>277</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -8959,13 +8967,13 @@
     </row>
     <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -8978,18 +8986,18 @@
         <v>1</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -9002,7 +9010,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -9060,7 +9068,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -9075,10 +9083,10 @@
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -9089,7 +9097,7 @@
         <v>251</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>252</v>
@@ -9113,7 +9121,7 @@
         <v>254</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>134</v>
@@ -9137,7 +9145,7 @@
         <v>256</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>85</v>
@@ -9161,7 +9169,7 @@
         <v>258</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -9185,7 +9193,7 @@
         <v>260</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -9198,7 +9206,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -9209,7 +9217,7 @@
         <v>262</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>252</v>
@@ -9222,7 +9230,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -9233,7 +9241,7 @@
         <v>264</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -9257,7 +9265,7 @@
         <v>266</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>267</v>
@@ -9278,14 +9286,14 @@
         <v>268</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="7" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>351</v>
@@ -9299,17 +9307,17 @@
     </row>
     <row r="11" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>529</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>531</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="7" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>351</v>

</xml_diff>

<commit_message>
Updated to current yaml formatting guidelines
</commit_message>
<xml_diff>
--- a/ARPES/tabular-to-yaml/mpes-nexus_metadata_parameters_reviewed.xlsx
+++ b/ARPES/tabular-to-yaml/mpes-nexus_metadata_parameters_reviewed.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Tommaso\Shared_Ubuntu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yolan\MPI\FHI\areab-appdef\ARPES\tabular-to-yaml\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA374BA-F089-49FF-A5FF-35F3F6B8F2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="784" firstSheet="8" activeTab="16"/>
+    <workbookView xWindow="60" yWindow="960" windowWidth="20085" windowHeight="10530" tabRatio="784" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NXentry" sheetId="1" r:id="rId1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="605">
   <si>
     <t>Name</t>
   </si>
@@ -2584,9 +2585,6 @@
   </si>
   <si>
     <t>NXnote</t>
-  </si>
-  <si>
-    <t>tipe:units</t>
   </si>
   <si>
     <t>NXentry:title</t>
@@ -3547,7 +3545,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3933,51 +3931,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -4001,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -4025,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -4049,7 +4047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -4073,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -4097,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>493</v>
       </c>
@@ -4121,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -4145,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -4169,7 +4167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -4193,7 +4191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -4217,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -4241,7 +4239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -4249,7 +4247,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -4265,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -4289,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -4297,7 +4295,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -4313,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
@@ -4321,7 +4319,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>17</v>
@@ -4337,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -4345,7 +4343,7 @@
         <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>18</v>
@@ -4361,7 +4359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
@@ -4385,7 +4383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -4416,59 +4414,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>269</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -4483,7 +4481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>270</v>
       </c>
@@ -4491,7 +4489,7 @@
         <v>271</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>82</v>
@@ -4506,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>272</v>
       </c>
@@ -4514,7 +4512,7 @@
         <v>273</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>82</v>
@@ -4529,19 +4527,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>351</v>
@@ -4553,19 +4551,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>492</v>
@@ -4577,7 +4575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>274</v>
       </c>
@@ -4585,7 +4583,7 @@
         <v>275</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
@@ -4600,15 +4598,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>277</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -4623,7 +4621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>278</v>
       </c>
@@ -4631,7 +4629,7 @@
         <v>279</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>85</v>
@@ -4646,16 +4644,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
     </row>
   </sheetData>
@@ -4664,53 +4662,52 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="29" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="28.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="6" customWidth="1"/>
     <col min="9" max="16384" width="29" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>280</v>
       </c>
@@ -4718,7 +4715,7 @@
         <v>281</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -4733,7 +4730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>282</v>
       </c>
@@ -4741,7 +4738,7 @@
         <v>283</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>182</v>
@@ -4756,7 +4753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>284</v>
       </c>
@@ -4764,7 +4761,7 @@
         <v>285</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>182</v>
@@ -4779,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>286</v>
       </c>
@@ -4787,7 +4784,7 @@
         <v>287</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>82</v>
@@ -4802,7 +4799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>288</v>
       </c>
@@ -4810,7 +4807,7 @@
         <v>289</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -4825,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>290</v>
       </c>
@@ -4833,7 +4830,7 @@
         <v>291</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -4848,7 +4845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>292</v>
       </c>
@@ -4856,7 +4853,7 @@
         <v>293</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -4871,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>294</v>
       </c>
@@ -4879,7 +4876,7 @@
         <v>295</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
@@ -4900,46 +4897,46 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="15.44140625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="4" width="15.42578125" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>296</v>
       </c>
@@ -4947,7 +4944,7 @@
         <v>297</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -4962,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>298</v>
       </c>
@@ -4970,7 +4967,7 @@
         <v>299</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -4985,7 +4982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>300</v>
       </c>
@@ -4993,7 +4990,7 @@
         <v>301</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>252</v>
@@ -5008,7 +5005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>302</v>
       </c>
@@ -5016,7 +5013,7 @@
         <v>303</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>85</v>
@@ -5031,7 +5028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>304</v>
       </c>
@@ -5039,7 +5036,7 @@
         <v>305</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>306</v>
@@ -5054,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>307</v>
       </c>
@@ -5062,7 +5059,7 @@
         <v>308</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
@@ -5077,11 +5074,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
@@ -5091,46 +5088,46 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="19" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
@@ -5153,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>311</v>
       </c>
@@ -5176,12 +5173,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>315</v>
@@ -5199,7 +5196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>316</v>
       </c>
@@ -5222,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>320</v>
       </c>
@@ -5245,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>323</v>
       </c>
@@ -5268,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>326</v>
       </c>
@@ -5291,7 +5288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>329</v>
       </c>
@@ -5314,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>332</v>
       </c>
@@ -5337,7 +5334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>335</v>
       </c>
@@ -5360,7 +5357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>338</v>
       </c>
@@ -5383,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>244</v>
       </c>
@@ -5406,7 +5403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>247</v>
       </c>
@@ -5429,7 +5426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>340</v>
       </c>
@@ -5452,7 +5449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>344</v>
       </c>
@@ -5475,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>347</v>
       </c>
@@ -5498,15 +5495,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>583</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>252</v>
@@ -5518,10 +5515,10 @@
         <v>1</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>350</v>
       </c>
@@ -5529,7 +5526,7 @@
         <v>352</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>186</v>
@@ -5544,15 +5541,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>186</v>
@@ -5564,10 +5561,10 @@
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>353</v>
       </c>
@@ -5590,15 +5587,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>343</v>
@@ -5610,10 +5607,10 @@
         <v>1</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>356</v>
       </c>
@@ -5636,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>359</v>
       </c>
@@ -5659,7 +5656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>362</v>
       </c>
@@ -5682,9 +5679,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>365</v>
@@ -5705,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>244</v>
       </c>
@@ -5728,7 +5725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>369</v>
       </c>
@@ -5751,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>372</v>
       </c>
@@ -5774,7 +5771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>375</v>
       </c>
@@ -5797,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>378</v>
       </c>
@@ -5820,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>381</v>
       </c>
@@ -5843,7 +5840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>384</v>
       </c>
@@ -5866,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>387</v>
       </c>
@@ -5889,7 +5886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>389</v>
       </c>
@@ -5913,13 +5910,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
     </row>
   </sheetData>
@@ -5928,46 +5925,46 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="21" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>392</v>
       </c>
@@ -5990,7 +5987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>395</v>
       </c>
@@ -6013,7 +6010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>398</v>
       </c>
@@ -6036,7 +6033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>401</v>
       </c>
@@ -6059,7 +6056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>404</v>
       </c>
@@ -6079,10 +6076,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>408</v>
       </c>
@@ -6102,10 +6099,10 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>411</v>
       </c>
@@ -6125,10 +6122,10 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>414</v>
       </c>
@@ -6148,10 +6145,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>417</v>
       </c>
@@ -6172,10 +6169,10 @@
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>420</v>
       </c>
@@ -6196,10 +6193,10 @@
         <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>423</v>
       </c>
@@ -6220,10 +6217,10 @@
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>426</v>
       </c>
@@ -6244,10 +6241,10 @@
         <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>429</v>
       </c>
@@ -6255,7 +6252,7 @@
         <v>430</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
@@ -6277,46 +6274,46 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="21" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>431</v>
       </c>
@@ -6339,7 +6336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>434</v>
       </c>
@@ -6362,7 +6359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>437</v>
       </c>
@@ -6385,7 +6382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>441</v>
       </c>
@@ -6405,10 +6402,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>444</v>
       </c>
@@ -6428,10 +6425,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>447</v>
       </c>
@@ -6451,34 +6448,34 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="4"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G9" s="4"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G10" s="4"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G11" s="4"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G12" s="4"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G13" s="4"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
@@ -6488,46 +6485,46 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="19.44140625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="4" width="19.42578125" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>431</v>
       </c>
@@ -6550,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>452</v>
       </c>
@@ -6573,7 +6570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>455</v>
       </c>
@@ -6596,7 +6593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>458</v>
       </c>
@@ -6616,10 +6613,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>461</v>
       </c>
@@ -6639,10 +6636,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>464</v>
       </c>
@@ -6665,7 +6662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>467</v>
       </c>
@@ -6685,7 +6682,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -6694,46 +6691,46 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="18.33203125" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="4" width="18.28515625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>431</v>
       </c>
@@ -6756,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>472</v>
       </c>
@@ -6776,10 +6773,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>475</v>
       </c>
@@ -6799,10 +6796,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>478</v>
       </c>
@@ -6822,10 +6819,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>481</v>
       </c>
@@ -6845,10 +6842,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>467</v>
       </c>
@@ -6871,7 +6868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>486</v>
       </c>
@@ -6900,51 +6897,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
@@ -6968,7 +6965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
@@ -6992,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>60</v>
       </c>
@@ -7016,7 +7013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>63</v>
       </c>
@@ -7040,7 +7037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>66</v>
       </c>
@@ -7064,7 +7061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>69</v>
       </c>
@@ -7088,7 +7085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>72</v>
       </c>
@@ -7119,51 +7116,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="23.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
@@ -7187,15 +7184,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -7211,7 +7208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -7241,52 +7238,52 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="22.109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="4"/>
-    <col min="8" max="8" width="12.44140625" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="4"/>
+    <col min="8" max="8" width="12.42578125" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
@@ -7309,7 +7306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>91</v>
       </c>
@@ -7332,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>93</v>
       </c>
@@ -7355,7 +7352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>95</v>
       </c>
@@ -7378,7 +7375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
@@ -7401,7 +7398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>102</v>
       </c>
@@ -7424,7 +7421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>105</v>
       </c>
@@ -7447,15 +7444,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>577</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>108</v>
@@ -7470,7 +7467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>110</v>
       </c>
@@ -7493,7 +7490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>114</v>
       </c>
@@ -7516,7 +7513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>118</v>
       </c>
@@ -7539,7 +7536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>121</v>
       </c>
@@ -7562,7 +7559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>124</v>
       </c>
@@ -7585,7 +7582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>128</v>
       </c>
@@ -7608,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>131</v>
       </c>
@@ -7631,7 +7628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>135</v>
       </c>
@@ -7654,7 +7651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>139</v>
       </c>
@@ -7677,7 +7674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>142</v>
       </c>
@@ -7698,10 +7695,10 @@
         <v>2</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>145</v>
       </c>
@@ -7724,7 +7721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>149</v>
       </c>
@@ -7747,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>152</v>
       </c>
@@ -7770,7 +7767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>155</v>
       </c>
@@ -7793,7 +7790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>158</v>
       </c>
@@ -7816,7 +7813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>162</v>
       </c>
@@ -7837,10 +7834,10 @@
         <v>2</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>165</v>
       </c>
@@ -7863,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>168</v>
       </c>
@@ -7886,7 +7883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>171</v>
       </c>
@@ -7916,52 +7913,52 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="4"/>
+    <col min="1" max="2" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="4"/>
     <col min="8" max="8" width="14" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="6"/>
+    <col min="9" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>174</v>
       </c>
@@ -7984,7 +7981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>102</v>
       </c>
@@ -8007,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>109</v>
       </c>
@@ -8030,15 +8027,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>82</v>
@@ -8053,15 +8050,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>565</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>566</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -8073,18 +8070,18 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>568</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>569</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
@@ -8096,10 +8093,10 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>183</v>
       </c>
@@ -8122,7 +8119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>139</v>
       </c>
@@ -8145,7 +8142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>189</v>
       </c>
@@ -8166,10 +8163,10 @@
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>192</v>
       </c>
@@ -8192,7 +8189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>195</v>
       </c>
@@ -8215,15 +8212,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>571</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>127</v>
@@ -8245,48 +8242,48 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16.5546875" style="6" customWidth="1"/>
-    <col min="5" max="7" width="8.88671875" style="6"/>
+    <col min="1" max="4" width="16.5703125" style="6" customWidth="1"/>
+    <col min="5" max="7" width="8.85546875" style="6"/>
     <col min="8" max="8" width="11" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="6"/>
+    <col min="9" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>128</v>
       </c>
@@ -8309,7 +8306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>200</v>
       </c>
@@ -8332,7 +8329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>203</v>
       </c>
@@ -8353,7 +8350,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -8362,46 +8359,46 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="15.88671875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="4" width="15.85546875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
@@ -8424,7 +8421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>208</v>
       </c>
@@ -8447,7 +8444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
@@ -8470,7 +8467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>212</v>
       </c>
@@ -8493,7 +8490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>215</v>
       </c>
@@ -8516,7 +8513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>218</v>
       </c>
@@ -8539,7 +8536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>221</v>
       </c>
@@ -8562,7 +8559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>224</v>
       </c>
@@ -8585,7 +8582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>228</v>
       </c>
@@ -8608,7 +8605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>231</v>
       </c>
@@ -8631,7 +8628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>234</v>
       </c>
@@ -8654,7 +8651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>238</v>
       </c>
@@ -8677,7 +8674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>241</v>
       </c>
@@ -8700,7 +8697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>244</v>
       </c>
@@ -8723,7 +8720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>247</v>
       </c>
@@ -8752,52 +8749,52 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>208</v>
       </c>
@@ -8805,7 +8802,7 @@
         <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -8821,7 +8818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>54</v>
       </c>
@@ -8829,7 +8826,7 @@
         <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -8845,15 +8842,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -8869,7 +8866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
@@ -8877,7 +8874,7 @@
         <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
@@ -8893,7 +8890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>80</v>
       </c>
@@ -8901,7 +8898,7 @@
         <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>82</v>
@@ -8917,7 +8914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>83</v>
       </c>
@@ -8925,7 +8922,7 @@
         <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
@@ -8941,7 +8938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>276</v>
       </c>
@@ -8949,7 +8946,7 @@
         <v>277</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -8965,15 +8962,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -8986,18 +8983,18 @@
         <v>1</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -9010,30 +9007,30 @@
         <v>1</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
@@ -9044,52 +9041,52 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="33" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="33" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="6"/>
-    <col min="4" max="4" width="29.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="6" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6" customWidth="1"/>
     <col min="9" max="16384" width="33" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>491</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>250</v>
       </c>
@@ -9097,7 +9094,7 @@
         <v>251</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>252</v>
@@ -9113,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>253</v>
       </c>
@@ -9121,7 +9118,7 @@
         <v>254</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>134</v>
@@ -9137,7 +9134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>255</v>
       </c>
@@ -9145,7 +9142,7 @@
         <v>256</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>85</v>
@@ -9161,7 +9158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>257</v>
       </c>
@@ -9169,7 +9166,7 @@
         <v>258</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -9185,7 +9182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>259</v>
       </c>
@@ -9193,7 +9190,7 @@
         <v>260</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -9206,10 +9203,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>261</v>
       </c>
@@ -9217,7 +9214,7 @@
         <v>262</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>252</v>
@@ -9230,10 +9227,10 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>263</v>
       </c>
@@ -9241,7 +9238,7 @@
         <v>264</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -9257,7 +9254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>265</v>
       </c>
@@ -9265,7 +9262,7 @@
         <v>266</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>267</v>
@@ -9281,19 +9278,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>351</v>
@@ -9305,19 +9302,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>351</v>
@@ -9329,23 +9326,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>

</xml_diff>

<commit_message>
Workaround badzipfile; fixed formatting.
</commit_message>
<xml_diff>
--- a/ARPES/tabular-to-yaml/mpes-nexus_metadata_parameters_reviewed.xlsx
+++ b/ARPES/tabular-to-yaml/mpes-nexus_metadata_parameters_reviewed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yolan\MPI\FHI\areab-appdef\ARPES\tabular-to-yaml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA374BA-F089-49FF-A5FF-35F3F6B8F2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6EDE3A-ADC7-4B4F-8F02-F38591D57D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="960" windowWidth="20085" windowHeight="10530" tabRatio="784" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="2100" windowWidth="20085" windowHeight="10530" tabRatio="784" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NXentry" sheetId="1" r:id="rId1"/>
@@ -963,9 +963,6 @@
     <t>NXentry:NXinstrument:NXpositioner:description</t>
   </si>
   <si>
-    <t xml:space="preserve">Type of manipulator: “Hexapod”, “Rod”, etc. </t>
-  </si>
-  <si>
     <r>
       <t>NXentry:NXinstrument:NXpositioner:</t>
     </r>
@@ -1257,9 +1254,6 @@
     <t>projection</t>
   </si>
   <si>
-    <t>The space projected in the angularly dispersive directions: “real” or “reciprocal”</t>
-  </si>
-  <si>
     <t>magnification</t>
   </si>
   <si>
@@ -1272,9 +1266,6 @@
     <t>field_aperture</t>
   </si>
   <si>
-    <t>“tof”, “hemispherical”, “cylindrical”, “mirror”, “retarding grid”, etc.</t>
-  </si>
-  <si>
     <t>pass_energy</t>
   </si>
   <si>
@@ -1296,9 +1287,6 @@
     <t>energy_scan_mode</t>
   </si>
   <si>
-    <t>“fixed” or “sweep”</t>
-  </si>
-  <si>
     <t>tof_distance</t>
   </si>
   <si>
@@ -1308,9 +1296,6 @@
     <t>spin_filter_type</t>
   </si>
   <si>
-    <t xml:space="preserve">Type of spin detector: “VLEED”, “SPLEED”, “Mott”, etc. </t>
-  </si>
-  <si>
     <t>spin_FoM</t>
   </si>
   <si>
@@ -1356,15 +1341,9 @@
     <t>amplifier_type</t>
   </si>
   <si>
-    <t>Type of electron amplifier: “MCP”, “channeltron”, etc.</t>
-  </si>
-  <si>
     <t>detector_type</t>
   </si>
   <si>
-    <t>Description of the detector type: “DLD”, “Phosphor+CCD”, “CMOS”.</t>
-  </si>
-  <si>
     <t>detector_voltage</t>
   </si>
   <si>
@@ -1481,9 +1460,6 @@
     <t>layer</t>
   </si>
   <si>
-    <t>Number of layers of the sample (e.g. “bulk”, “monolayer”, “pentalayer”, etc.)</t>
-  </si>
-  <si>
     <r>
       <t>NXentry:NXsample:</t>
     </r>
@@ -1539,9 +1515,6 @@
     <t>chem_id_cas</t>
   </si>
   <si>
-    <t>CAS registry number of the sample’s chemical content.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">NXentry:NXsample: </t>
     </r>
@@ -1577,9 +1550,6 @@
     <t>gas</t>
   </si>
   <si>
-    <t>Gases might be fluxed on the surface for various reasons. Chemical designation, or “residual”.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">NXentry:NXsample: </t>
     </r>
@@ -1725,9 +1695,6 @@
   </si>
   <si>
     <t>preparation_method</t>
-  </si>
-  <si>
-    <t>E.g. “UHV cleave”, “sputtering and annealing”, etc.</t>
   </si>
   <si>
     <r>
@@ -3540,6 +3507,39 @@
       </rPr>
       <t>NXelectronanalyser:name:\@short_name</t>
     </r>
+  </si>
+  <si>
+    <t>CAS registry number of the sample's chemical content.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of manipulator: "Hexapod", "Rod", etc. </t>
+  </si>
+  <si>
+    <t>"fixed" or "sweep"</t>
+  </si>
+  <si>
+    <t>The space projected in the angularly dispersive directions: "real" or "reciprocal"</t>
+  </si>
+  <si>
+    <t>"tof", "hemispherical", "cylindrical", "mirror", "retarding grid", etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of spin detector: "VLEED", "SPLEED", "Mott", etc. </t>
+  </si>
+  <si>
+    <t>Type of electron amplifier: "MCP", "channeltron", etc.</t>
+  </si>
+  <si>
+    <t>Description of the detector type: "DLD", "Phosphor+CCD", "CMOS".</t>
+  </si>
+  <si>
+    <t>Number of layers of the sample (e.g. "bulk", "monolayer", "pentalayer", etc.)</t>
+  </si>
+  <si>
+    <t>Gases might be fluxed on the surface for various reasons. Chemical designation, or "residual".</t>
+  </si>
+  <si>
+    <t>E.g. "UHV cleave", "sputtering and annealing", etc.</t>
   </si>
 </sst>
 </file>
@@ -3954,25 +3954,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -3990,7 +3990,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -4038,7 +4038,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="3" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="3" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -4097,20 +4097,20 @@
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -4158,7 +4158,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="3" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -4247,14 +4247,14 @@
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -4295,14 +4295,14 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -4319,14 +4319,14 @@
         <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -4343,14 +4343,14 @@
         <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -4398,7 +4398,7 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -4437,42 +4437,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>269</v>
+        <v>598</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -4483,19 +4483,19 @@
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -4506,19 +4506,19 @@
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -4529,20 +4529,20 @@
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -4553,20 +4553,20 @@
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>539</v>
+        <v>528</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -4577,19 +4577,19 @@
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>540</v>
+        <v>529</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -4600,19 +4600,19 @@
     </row>
     <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>543</v>
+        <v>532</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -4623,19 +4623,19 @@
     </row>
     <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>544</v>
+        <v>533</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -4686,42 +4686,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>281</v>
+        <v>599</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -4732,19 +4732,19 @@
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -4755,19 +4755,19 @@
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>547</v>
+        <v>536</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -4778,19 +4778,19 @@
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>548</v>
+        <v>537</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -4801,19 +4801,19 @@
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>549</v>
+        <v>538</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -4824,19 +4824,19 @@
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -4847,19 +4847,19 @@
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -4870,19 +4870,19 @@
     </row>
     <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -4915,42 +4915,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>297</v>
+        <v>600</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -4961,19 +4961,19 @@
     </row>
     <row r="3" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>299</v>
+        <v>601</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -4984,19 +4984,19 @@
     </row>
     <row r="4" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -5007,19 +5007,19 @@
     </row>
     <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -5030,19 +5030,19 @@
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -5053,19 +5053,19 @@
     </row>
     <row r="7" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -5091,8 +5091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5106,25 +5106,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -5132,16 +5132,16 @@
         <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -5152,19 +5152,19 @@
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -5175,19 +5175,19 @@
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -5198,19 +5198,19 @@
     </row>
     <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -5221,19 +5221,19 @@
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -5244,19 +5244,19 @@
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>324</v>
+        <v>602</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -5267,19 +5267,19 @@
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -5290,19 +5290,19 @@
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -5313,19 +5313,19 @@
     </row>
     <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -5336,19 +5336,19 @@
     </row>
     <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>336</v>
+        <v>594</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -5359,19 +5359,19 @@
     </row>
     <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -5382,19 +5382,19 @@
     </row>
     <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -5405,19 +5405,19 @@
     </row>
     <row r="14" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -5428,19 +5428,19 @@
     </row>
     <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -5451,19 +5451,19 @@
     </row>
     <row r="16" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>345</v>
+        <v>603</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -5474,19 +5474,19 @@
     </row>
     <row r="17" spans="1:8" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -5497,42 +5497,42 @@
     </row>
     <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G18" s="4">
         <v>1</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -5543,42 +5543,42 @@
     </row>
     <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G20" s="4">
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G21" s="4">
         <v>0</v>
@@ -5589,42 +5589,42 @@
     </row>
     <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G22" s="4">
         <v>1</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G23" s="4">
         <v>0</v>
@@ -5635,19 +5635,19 @@
     </row>
     <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G24" s="4">
         <v>0</v>
@@ -5658,19 +5658,19 @@
     </row>
     <row r="25" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G25" s="4">
         <v>0</v>
@@ -5681,19 +5681,19 @@
     </row>
     <row r="26" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G26" s="4">
         <v>0</v>
@@ -5704,19 +5704,19 @@
     </row>
     <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G27" s="4">
         <v>0</v>
@@ -5727,19 +5727,19 @@
     </row>
     <row r="28" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G28" s="4">
         <v>0</v>
@@ -5750,19 +5750,19 @@
     </row>
     <row r="29" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>373</v>
+        <v>604</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G29" s="4">
         <v>0</v>
@@ -5773,19 +5773,19 @@
     </row>
     <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G30" s="4">
         <v>0</v>
@@ -5796,19 +5796,19 @@
     </row>
     <row r="31" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G31" s="4">
         <v>0</v>
@@ -5819,19 +5819,19 @@
     </row>
     <row r="32" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G32" s="4">
         <v>0</v>
@@ -5842,19 +5842,19 @@
     </row>
     <row r="33" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G33" s="4">
         <v>0</v>
@@ -5865,19 +5865,19 @@
     </row>
     <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G34" s="4">
         <v>0</v>
@@ -5888,20 +5888,20 @@
     </row>
     <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G35" s="4">
         <v>0</v>
@@ -5943,42 +5943,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -5989,19 +5989,19 @@
     </row>
     <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -6012,19 +6012,19 @@
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -6035,19 +6035,19 @@
     </row>
     <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -6058,208 +6058,208 @@
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4" t="s">
         <v>206</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G10" s="4">
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="s">
         <v>206</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="4" t="s">
         <v>206</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G12" s="4">
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="4" t="s">
         <v>206</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G13" s="4">
         <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
         <v>206</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -6277,7 +6277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H7"/>
     </sheetView>
   </sheetViews>
@@ -6292,42 +6292,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -6338,19 +6338,19 @@
     </row>
     <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -6361,19 +6361,19 @@
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -6384,71 +6384,71 @@
     </row>
     <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6503,42 +6503,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -6549,19 +6549,19 @@
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -6572,19 +6572,19 @@
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -6595,65 +6595,65 @@
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -6664,25 +6664,25 @@
     </row>
     <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
     </row>
   </sheetData>
@@ -6709,42 +6709,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -6755,111 +6755,111 @@
     </row>
     <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>1</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -6870,19 +6870,19 @@
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -6920,25 +6920,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -6980,7 +6980,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -7004,7 +7004,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -7028,7 +7028,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -7052,7 +7052,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -7076,7 +7076,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -7100,7 +7100,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -7139,25 +7139,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -7175,7 +7175,7 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -7186,20 +7186,20 @@
     </row>
     <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -7223,7 +7223,7 @@
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -7262,25 +7262,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -7297,7 +7297,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -7314,13 +7314,13 @@
         <v>92</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -7337,13 +7337,13 @@
         <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -7366,7 +7366,7 @@
         <v>82</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -7389,7 +7389,7 @@
         <v>101</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -7412,7 +7412,7 @@
         <v>82</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -7435,7 +7435,7 @@
         <v>108</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -7446,19 +7446,19 @@
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -7481,7 +7481,7 @@
         <v>113</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -7504,7 +7504,7 @@
         <v>117</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -7527,7 +7527,7 @@
         <v>85</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -7550,7 +7550,7 @@
         <v>85</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -7573,7 +7573,7 @@
         <v>127</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -7596,7 +7596,7 @@
         <v>82</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -7619,7 +7619,7 @@
         <v>134</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -7642,7 +7642,7 @@
         <v>138</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -7665,7 +7665,7 @@
         <v>18</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -7689,13 +7689,13 @@
         <v>206</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G19" s="4">
         <v>2</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -7712,7 +7712,7 @@
         <v>148</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -7735,7 +7735,7 @@
         <v>18</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G21" s="4">
         <v>0</v>
@@ -7758,7 +7758,7 @@
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G22" s="4">
         <v>0</v>
@@ -7781,7 +7781,7 @@
         <v>6</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G23" s="4">
         <v>0</v>
@@ -7804,7 +7804,7 @@
         <v>161</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G24" s="4">
         <v>0</v>
@@ -7828,13 +7828,13 @@
         <v>206</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G25" s="4">
         <v>2</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
@@ -7851,7 +7851,7 @@
         <v>18</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G26" s="4">
         <v>0</v>
@@ -7874,7 +7874,7 @@
         <v>148</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G27" s="4">
         <v>0</v>
@@ -7897,7 +7897,7 @@
         <v>148</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G28" s="4">
         <v>0</v>
@@ -7937,25 +7937,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -7972,7 +7972,7 @@
         <v>85</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -7995,7 +7995,7 @@
         <v>82</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -8018,7 +8018,7 @@
         <v>108</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -8029,19 +8029,19 @@
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>563</v>
+        <v>552</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -8052,48 +8052,48 @@
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>564</v>
+        <v>553</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -8110,7 +8110,7 @@
         <v>186</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -8133,7 +8133,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -8157,13 +8157,13 @@
         <v>206</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G10" s="4">
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -8180,7 +8180,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -8203,7 +8203,7 @@
         <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -8217,16 +8217,16 @@
         <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>569</v>
+        <v>558</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -8262,25 +8262,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -8297,7 +8297,7 @@
         <v>82</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -8320,7 +8320,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -8344,13 +8344,13 @@
         <v>206</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G4" s="4">
         <v>2</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -8377,25 +8377,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -8412,7 +8412,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -8435,7 +8435,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -8449,16 +8449,16 @@
         <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -8469,19 +8469,19 @@
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -8492,19 +8492,19 @@
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -8515,19 +8515,19 @@
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -8538,19 +8538,19 @@
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -8561,19 +8561,19 @@
     </row>
     <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -8584,19 +8584,19 @@
     </row>
     <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -8607,19 +8607,19 @@
     </row>
     <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -8630,19 +8630,19 @@
     </row>
     <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>237</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -8653,19 +8653,19 @@
     </row>
     <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -8676,19 +8676,19 @@
     </row>
     <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -8699,19 +8699,19 @@
     </row>
     <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -8722,19 +8722,19 @@
     </row>
     <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -8773,25 +8773,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -8802,14 +8802,14 @@
         <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -8826,14 +8826,14 @@
         <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -8844,20 +8844,20 @@
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -8874,14 +8874,14 @@
         <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -8898,14 +8898,14 @@
         <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>82</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -8922,14 +8922,14 @@
         <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -8940,20 +8940,20 @@
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -8964,50 +8964,50 @@
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>579</v>
+        <v>568</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -9065,43 +9065,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -9112,20 +9112,20 @@
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -9136,20 +9136,20 @@
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -9160,20 +9160,20 @@
     </row>
     <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -9184,68 +9184,68 @@
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>264</v>
+        <v>597</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -9256,20 +9256,20 @@
     </row>
     <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -9280,20 +9280,20 @@
     </row>
     <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="7" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -9304,20 +9304,20 @@
     </row>
     <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="7" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>

</xml_diff>